<commit_message>
updating Muus Data Log.xlsx with corrected filenames, masses and flow rates
</commit_message>
<xml_diff>
--- a/RMR_Results.xlsx
+++ b/RMR_Results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="75">
   <si>
     <t>filename</t>
   </si>
@@ -125,18 +125,6 @@
     <t>32</t>
   </si>
   <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
     <t>Gr1 Muus 1800-2  7day-8-2-21.txt</t>
   </si>
   <si>
@@ -161,9 +149,6 @@
     <t>gr2muus1000-2 7-26-21.txt</t>
   </si>
   <si>
-    <t>gr2muus1000-2 7-26-21(1).txt</t>
-  </si>
-  <si>
     <t>gr2muus1800 7day 7-19-21.txt</t>
   </si>
   <si>
@@ -179,9 +164,6 @@
     <t>gr3 muus 1000 7-20-21.txt</t>
   </si>
   <si>
-    <t>gr3 muus 1000 7-20-21(1).txt</t>
-  </si>
-  <si>
     <t>gr3 muus 1000-2 7day 7-26-21.txt</t>
   </si>
   <si>
@@ -194,13 +176,7 @@
     <t>gr3 muus 1800 7-12-21.txt</t>
   </si>
   <si>
-    <t>gr3 muus 1800 7-12-21(1).txt</t>
-  </si>
-  <si>
     <t>gr3 muus 1800 7day-7-19-21.txt</t>
-  </si>
-  <si>
-    <t>gr3 muus 1800 7day-7-19-21(1).txt</t>
   </si>
   <si>
     <t>GR4MUUS1000-2-7-26-21-ch1.txt</t>
@@ -334,10 +310,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D2" t="n">
         <v>2.5</v>
@@ -354,10 +330,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D3" t="n">
         <v>20.6</v>
@@ -374,10 +350,10 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D4" t="n">
         <v>20.6</v>
@@ -394,10 +370,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D5" t="n">
         <v>30.8</v>
@@ -414,10 +390,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D6" t="n">
         <v>30.8</v>
@@ -434,10 +410,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D7" t="n">
         <v>2.5</v>
@@ -454,10 +430,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D8" t="n">
         <v>35.0</v>
@@ -474,10 +450,10 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D9" t="n">
         <v>35.0</v>
@@ -494,19 +470,19 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="D10" t="n">
-        <v>35.0</v>
+        <v>16.8</v>
       </c>
       <c r="E10" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="F10" t="e">
-        <v>#N/A</v>
+        <v>1800.0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2.878785297965981</v>
       </c>
     </row>
     <row r="11">
@@ -514,19 +490,19 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="D11" t="n">
-        <v>16.8</v>
+        <v>2.6</v>
       </c>
       <c r="E11" t="n">
         <v>1800.0</v>
       </c>
       <c r="F11" t="n">
-        <v>2.878785297965981</v>
+        <v>20.512713859416444</v>
       </c>
     </row>
     <row r="12">
@@ -534,10 +510,10 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D12" t="n">
         <v>2.6</v>
@@ -546,7 +522,7 @@
         <v>1800.0</v>
       </c>
       <c r="F12" t="n">
-        <v>20.512713859416444</v>
+        <v>21.53399145462287</v>
       </c>
     </row>
     <row r="13">
@@ -554,19 +530,19 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="D13" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="E13" t="n">
-        <v>1800.0</v>
+        <v>70.0</v>
+      </c>
+      <c r="E13" t="e">
+        <v>#N/A</v>
       </c>
       <c r="F13" t="n">
-        <v>21.53399145462287</v>
+        <v>0.4047610012843986</v>
       </c>
     </row>
     <row r="14">
@@ -574,19 +550,19 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D14" t="n">
-        <v>70.0</v>
-      </c>
-      <c r="E14" t="e">
-        <v>#N/A</v>
+        <v>21.6</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1000.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.4047610012843986</v>
+        <v>26.60150377057981</v>
       </c>
     </row>
     <row r="15">
@@ -594,10 +570,10 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D15" t="n">
         <v>21.6</v>
@@ -606,7 +582,7 @@
         <v>1000.0</v>
       </c>
       <c r="F15" t="n">
-        <v>26.60150377057981</v>
+        <v>1.6166100623885917</v>
       </c>
     </row>
     <row r="16">
@@ -614,19 +590,19 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="D16" t="n">
-        <v>21.6</v>
+        <v>16.9</v>
       </c>
       <c r="E16" t="n">
-        <v>1000.0</v>
+        <v>1800.0</v>
       </c>
       <c r="F16" t="n">
-        <v>26.60150377057981</v>
+        <v>1.8751649422561198</v>
       </c>
     </row>
     <row r="17">
@@ -634,19 +610,19 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D17" t="n">
-        <v>21.6</v>
+        <v>16.9</v>
       </c>
       <c r="E17" t="n">
-        <v>1000.0</v>
+        <v>1800.0</v>
       </c>
       <c r="F17" t="n">
-        <v>1.6166100623885917</v>
+        <v>2.4225296644488474</v>
       </c>
     </row>
     <row r="18">
@@ -654,19 +630,19 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="D18" t="n">
-        <v>16.9</v>
+        <v>70.0</v>
       </c>
       <c r="E18" t="n">
         <v>1800.0</v>
       </c>
       <c r="F18" t="n">
-        <v>1.8751649422561198</v>
+        <v>1.7253897049808429</v>
       </c>
     </row>
     <row r="19">
@@ -674,19 +650,19 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="D19" t="n">
-        <v>16.9</v>
+        <v>70.0</v>
       </c>
       <c r="E19" t="n">
         <v>1800.0</v>
       </c>
       <c r="F19" t="n">
-        <v>2.4225296644488474</v>
+        <v>1.9351934399102106</v>
       </c>
     </row>
     <row r="20">
@@ -694,19 +670,19 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D20" t="n">
-        <v>70.0</v>
+        <v>15.5</v>
       </c>
       <c r="E20" t="n">
-        <v>1800.0</v>
+        <v>1000.0</v>
       </c>
       <c r="F20" t="n">
-        <v>1.7253897049808429</v>
+        <v>3.504599061636401</v>
       </c>
     </row>
     <row r="21">
@@ -714,19 +690,19 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D21" t="n">
-        <v>70.0</v>
+        <v>15.5</v>
       </c>
       <c r="E21" t="n">
-        <v>1800.0</v>
+        <v>1000.0</v>
       </c>
       <c r="F21" t="n">
-        <v>1.7253897049808429</v>
+        <v>2.6116131743930984</v>
       </c>
     </row>
     <row r="22">
@@ -734,19 +710,19 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D22" t="n">
-        <v>70.0</v>
+        <v>15.5</v>
       </c>
       <c r="E22" t="n">
         <v>1800.0</v>
       </c>
       <c r="F22" t="n">
-        <v>1.9351934399102106</v>
+        <v>8.57191893437052</v>
       </c>
     </row>
     <row r="23">
@@ -754,19 +730,19 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="D23" t="n">
-        <v>70.0</v>
+        <v>41.3</v>
       </c>
       <c r="E23" t="n">
         <v>1800.0</v>
       </c>
       <c r="F23" t="n">
-        <v>1.9351934399102106</v>
+        <v>2.174192166865828</v>
       </c>
     </row>
     <row r="24">
@@ -774,19 +750,19 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D24" t="n">
-        <v>15.5</v>
+        <v>27.5</v>
       </c>
       <c r="E24" t="n">
-        <v>1000.0</v>
+        <v>1800.0</v>
       </c>
       <c r="F24" t="n">
-        <v>3.504599061636401</v>
+        <v>1.9267980832143867</v>
       </c>
     </row>
     <row r="25">
@@ -794,19 +770,19 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="D25" t="n">
-        <v>15.5</v>
+        <v>27.5</v>
       </c>
       <c r="E25" t="n">
-        <v>1000.0</v>
+        <v>1800.0</v>
       </c>
       <c r="F25" t="n">
-        <v>2.6116131743930984</v>
+        <v>2.4912386837390432</v>
       </c>
     </row>
     <row r="26">
@@ -814,19 +790,19 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D26" t="n">
-        <v>15.5</v>
+        <v>13.0</v>
       </c>
       <c r="E26" t="n">
-        <v>1800.0</v>
+        <v>1000.0</v>
       </c>
       <c r="F26" t="n">
-        <v>8.57191893437052</v>
+        <v>1.5277540870569055</v>
       </c>
     </row>
     <row r="27">
@@ -834,19 +810,19 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="D27" t="n">
-        <v>41.3</v>
+        <v>4.4</v>
       </c>
       <c r="E27" t="n">
-        <v>1800.0</v>
+        <v>1000.0</v>
       </c>
       <c r="F27" t="n">
-        <v>2.174192166865828</v>
+        <v>3.8065838709866746</v>
       </c>
     </row>
     <row r="28">
@@ -854,19 +830,19 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D28" t="n">
-        <v>27.5</v>
+        <v>13.0</v>
       </c>
       <c r="E28" t="n">
-        <v>1800.0</v>
+        <v>1000.0</v>
       </c>
       <c r="F28" t="n">
-        <v>1.9267980832143867</v>
+        <v>3.7820826019201834</v>
       </c>
     </row>
     <row r="29">
@@ -874,19 +850,19 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D29" t="n">
-        <v>27.5</v>
+        <v>4.4</v>
       </c>
       <c r="E29" t="n">
-        <v>1800.0</v>
+        <v>1000.0</v>
       </c>
       <c r="F29" t="n">
-        <v>2.4912386837390432</v>
+        <v>6.942437886686441</v>
       </c>
     </row>
     <row r="30">
@@ -894,19 +870,19 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D30" t="n">
-        <v>13.0</v>
+        <v>36.3</v>
       </c>
       <c r="E30" t="n">
         <v>1000.0</v>
       </c>
       <c r="F30" t="n">
-        <v>1.5277540870569055</v>
+        <v>1.3460007971381225</v>
       </c>
     </row>
     <row r="31">
@@ -914,19 +890,19 @@
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D31" t="n">
-        <v>4.4</v>
+        <v>25.1</v>
       </c>
       <c r="E31" t="n">
         <v>1000.0</v>
       </c>
       <c r="F31" t="n">
-        <v>3.8065838709866746</v>
+        <v>2.8036070307370924</v>
       </c>
     </row>
     <row r="32">
@@ -934,10 +910,10 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D32" t="n">
         <v>13.0</v>
@@ -946,7 +922,7 @@
         <v>1000.0</v>
       </c>
       <c r="F32" t="n">
-        <v>3.7820826019201834</v>
+        <v>1.5277540870569055</v>
       </c>
     </row>
     <row r="33">
@@ -954,10 +930,10 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D33" t="n">
         <v>4.4</v>
@@ -966,86 +942,6 @@
         <v>1000.0</v>
       </c>
       <c r="F33" t="n">
-        <v>6.942437886686441</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" t="n">
-        <v>36.3</v>
-      </c>
-      <c r="E34" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="F34" t="n">
-        <v>1.3460007971381225</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" t="n">
-        <v>25.1</v>
-      </c>
-      <c r="E35" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="F35" t="n">
-        <v>2.8036070307370924</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36" t="n">
-        <v>13.0</v>
-      </c>
-      <c r="E36" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="F36" t="n">
-        <v>1.5277540870569055</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="E37" t="n">
-        <v>1000.0</v>
-      </c>
-      <c r="F37" t="n">
         <v>3.8065838709866746</v>
       </c>
     </row>

</xml_diff>